<commit_message>
Update Portfolio matrix for MITBMUN22.xlsx
</commit_message>
<xml_diff>
--- a/assets/files/Portfolio matrix for MITBMUN22.xlsx
+++ b/assets/files/Portfolio matrix for MITBMUN22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mitbmun2022.github.io\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CBA2E6-7572-4E71-BD07-431E0CBE437E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E01EC99-B07B-48A3-BC3F-6DBFA38D5E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C6E23F96-2086-4AF0-8BC8-641864C3F5A0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C6E23F96-2086-4AF0-8BC8-641864C3F5A0}"/>
   </bookViews>
   <sheets>
     <sheet name="UNHRC" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>hi</t>
   </si>
@@ -147,13 +147,193 @@
   </si>
   <si>
     <t>North Korea</t>
+  </si>
+  <si>
+    <t>Narendra  Modi</t>
+  </si>
+  <si>
+    <t>Amit shah</t>
+  </si>
+  <si>
+    <t>Sonia gandhi(INC)</t>
+  </si>
+  <si>
+    <t>akhilesh</t>
+  </si>
+  <si>
+    <t>mulayam singh</t>
+  </si>
+  <si>
+    <t>shashi Tharoor</t>
+  </si>
+  <si>
+    <t>yogi adityanath</t>
+  </si>
+  <si>
+    <t>Deepak adhikari (AITC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abhishek Banerjee </t>
+  </si>
+  <si>
+    <t>Arvind Kejriwal</t>
+  </si>
+  <si>
+    <t>Smriti Zubin Irani (BJP)</t>
+  </si>
+  <si>
+    <t>Asaddudin Owaisi (AIMIM)</t>
+  </si>
+  <si>
+    <t>Jaleel Syed Imtiaz (AIMIM)</t>
+  </si>
+  <si>
+    <t>Maddila Gurumoorthy (YSRC)</t>
+  </si>
+  <si>
+    <t>YS jagan Mohan Reddy (YSRC)</t>
+  </si>
+  <si>
+    <t>Gautam Gambhir (BJP)</t>
+  </si>
+  <si>
+    <t>Rahul Gandhi (inc)</t>
+  </si>
+  <si>
+    <t>Manish Tiwari (inc)</t>
+  </si>
+  <si>
+    <t>Nusrat Jahan Ruhi (AITC)</t>
+  </si>
+  <si>
+    <t>Sudipp Bandyopadhyay (AITC)</t>
+  </si>
+  <si>
+    <t>Gajanan Chandrakant Kirtikar (SS)</t>
+  </si>
+  <si>
+    <t>Uddhav Thackeray (SS)</t>
+  </si>
+  <si>
+    <t>Dileshwar Kamait (JD)</t>
+  </si>
+  <si>
+    <t>Vijay Kumar (JD)</t>
+  </si>
+  <si>
+    <t>Kavita Singh (JD)</t>
+  </si>
+  <si>
+    <t>Bhartruhari Mahtab (BJD)</t>
+  </si>
+  <si>
+    <t>Pinaki Misra (BJD)</t>
+  </si>
+  <si>
+    <t>Rajashree Mallick (BJD)</t>
+  </si>
+  <si>
+    <t>Shyam singh yadav (BSP)</t>
+  </si>
+  <si>
+    <t>Sangeeta Azad(BSP)</t>
+  </si>
+  <si>
+    <t>Abu haseem khan Choudhary (INC)</t>
+  </si>
+  <si>
+    <t>Jasbeer singh gill (INC)</t>
+  </si>
+  <si>
+    <t>Navneet Ravi Rana (ind.)</t>
+  </si>
+  <si>
+    <t>Sumalatha Ambareesh (ind)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mamata Banerjee </t>
+  </si>
+  <si>
+    <t>Dr. Manmohan singh</t>
+  </si>
+  <si>
+    <t>Jaya Bachchan</t>
+  </si>
+  <si>
+    <t>Shivraj Singh Chouhan</t>
+  </si>
+  <si>
+    <t>Ashok Gehlot</t>
+  </si>
+  <si>
+    <t>M.K Stalin</t>
+  </si>
+  <si>
+    <t>Naveen Patnaik</t>
+  </si>
+  <si>
+    <t>Jairam Thakur</t>
+  </si>
+  <si>
+    <t>Bhupendra Patel</t>
+  </si>
+  <si>
+    <t>Pema Khandu</t>
+  </si>
+  <si>
+    <t>Himanta Biswa Sarma</t>
+  </si>
+  <si>
+    <t>Bhupesh Bhagel</t>
+  </si>
+  <si>
+    <t>Parmod Sawant</t>
+  </si>
+  <si>
+    <t>Manohar Lal</t>
+  </si>
+  <si>
+    <t>Hemant Soren</t>
+  </si>
+  <si>
+    <t>Basavaraj Bommai</t>
+  </si>
+  <si>
+    <t>Pinarai Vijayan</t>
+  </si>
+  <si>
+    <t>N.Biren Singh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conrad Kongkal Sangam </t>
+  </si>
+  <si>
+    <t>N. Rangaswamy</t>
+  </si>
+  <si>
+    <t>Charanjit Singh Channi</t>
+  </si>
+  <si>
+    <t>Piyush Goyal</t>
+  </si>
+  <si>
+    <t>Mallikarjun Kharge</t>
+  </si>
+  <si>
+    <t>Anand Sharma</t>
+  </si>
+  <si>
+    <t>Mukhtar Abbas Naqvi</t>
+  </si>
+  <si>
+    <t>Portfolia name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +359,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -234,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -251,6 +439,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,12 +772,316 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1AC6D96-FB2F-4487-BDE5-2F1C11B109EF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A60"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="32.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -598,7 +1091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7ABB783-17DA-48E8-AAFE-38E56D1CE283}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>